<commit_message>
still on background, fixed graphs to be in terms of radians etc. added nice graphs to metrics. have wrote a fair bit now though... just got to hope someone likes it!
</commit_message>
<xml_diff>
--- a/Report/Misc/Test Output/Arduino Test/Graphs.xlsx
+++ b/Report/Misc/Test Output/Arduino Test/Graphs.xlsx
@@ -67,64 +67,64 @@
     <t xml:space="preserve">0.994861,-0.043369,-0.091498,105.507744,0.043767,0.999039,0.002350,-5.961123,0.091308,-0.006343,0.995803,-3.172411,0.000000,0.000000,0.000000,1.000000</t>
   </si>
   <si>
-    <t xml:space="preserve">0, 102</t>
+    <t xml:space="preserve">0, 17</t>
   </si>
   <si>
-    <t xml:space="preserve">0.996163,-0.087481,-0.020706,17.291636,0.088763,0.993708,0.071039,-101.650093,0.014362,-0.072597,0.997369,-4.618966,0.000000,0.000000,0.000000,1.000000</t>
+    <t xml:space="preserve">0.038663,0.999155,-0.015959,365.957153,-0.961273,0.032822,-0.273733,464.012634,-0.272972,0.025922,0.961686,65.647797,0.000000,0.000000,0.000000,1.000000</t>
   </si>
   <si>
-    <t xml:space="preserve">0, 202</t>
+    <t xml:space="preserve">0, 32</t>
   </si>
   <si>
-    <t xml:space="preserve">0.798334,0.602807,0.012228,113.360664,-0.602592,0.797144,0.048667,87.048065,0.019587,-0.046226,0.998988,-7.875946,0.000000,0.000000,0.000000,1.000000</t>
+    <t xml:space="preserve">0.035316,0.992411,0.118269,165.083847,-0.998801,0.030794,0.039766,86.358902,0.035821,-0.119529,0.992215,-10.808743,0.000000,0.000000,0.000000,1.000000</t>
   </si>
   <si>
-    <t xml:space="preserve">0, 302</t>
+    <t xml:space="preserve">0, 47</t>
   </si>
   <si>
-    <t xml:space="preserve">0.635223,-0.773382,0.009403,36.035782,0.770917,0.634262,0.070284,-247.709656,-0.060280,-0.037413,0.997901,11.493330,0.000000,0.000000,0.000000,1.000000</t>
+    <t xml:space="preserve">-0.953780,-0.295352,-0.057124,377.185303,0.293666,-0.955319,0.036029,-272.454346,-0.065209,0.017584,0.997762,9.643250,0.000000,0.000000,0.000000,1.000000</t>
   </si>
   <si>
-    <t xml:space="preserve">0, 402</t>
+    <t xml:space="preserve">0, 62</t>
   </si>
   <si>
-    <t xml:space="preserve">-0.879993,-0.477127,0.003769,277.117615,0.477078,-0.880260,0.003191,-243.577972,0.001797,0.004566,1.000556,-0.079196,0.000000,0.000000,0.000000,1.000000</t>
+    <t xml:space="preserve">-0.959883,-0.266864,-0.087477,418.824707,0.263917,-0.963655,0.043828,-275.484131,-0.095987,0.018979,0.995269,15.784320,0.000000,0.000000,0.000000,1.000000</t>
   </si>
   <si>
-    <t xml:space="preserve">0, 502</t>
+    <t xml:space="preserve">0, 77</t>
   </si>
   <si>
-    <t xml:space="preserve">0.963433,0.271132,-0.027870,80.513031,-0.266420,0.958717,0.114203,-55.344742,0.057634,-0.102612,0.993820,-10.107821,0.000000,0.000000,0.000000,1.000000</t>
+    <t xml:space="preserve">-0.769638,0.635560,-0.063222,483.649475,-0.638100,-0.769464,0.032367,-113.468079,-0.028070,0.065245,0.997565,13.690338,0.000000,0.000000,0.000000,1.000000</t>
   </si>
   <si>
-    <t xml:space="preserve">0, 602</t>
+    <t xml:space="preserve">0, 92</t>
   </si>
   <si>
-    <t xml:space="preserve">1.001365,0.020552,0.000337,2.415299,-0.020678,0.999511,0.068330,-50.014515,0.001087,-0.068459,0.998602,-5.052285,0.000000,0.000000,0.000000,1.000000</t>
+    <t xml:space="preserve">0.950592,-0.308990,-0.035646,28.411476,0.310747,0.948474,0.064858,-135.075256,0.013770,-0.072724,0.997360,-3.179838,0.000000,0.000000,0.000000,1.000000</t>
   </si>
   <si>
-    <t xml:space="preserve">0, 702</t>
+    <t xml:space="preserve">0, 107</t>
   </si>
   <si>
-    <t xml:space="preserve">-0.974733,-0.220065,-0.071898,406.981018,0.221540,-0.977623,-0.012048,-207.154755,-0.067511,-0.027716,0.998395,4.413674,0.000000,0.000000,0.000000,1.000000</t>
+    <t xml:space="preserve">0.960013,0.280538,-0.011149,51.365917,-0.280488,0.960046,0.005101,37.332489,0.012137,-0.001773,1.000038,-0.523544,0.000000,0.000000,0.000000,1.000000</t>
   </si>
   <si>
-    <t xml:space="preserve">0, 802</t>
+    <t xml:space="preserve">0, 122</t>
   </si>
   <si>
-    <t xml:space="preserve">-0.692475,0.716978,-0.106717,541.121033,-0.724281,-0.686231,0.094788,-150.694366,-0.005279,0.142779,0.990955,23.794020,0.000000,0.000000,0.000000,1.000000</t>
+    <t xml:space="preserve">0.838037,-0.545962,-0.008549,-4.256080,0.541376,0.828682,0.143686,-313.379272,-0.071354,-0.125028,0.989705,9.232149,0.000000,0.000000,0.000000,1.000000</t>
   </si>
   <si>
-    <t xml:space="preserve">0, 902</t>
+    <t xml:space="preserve">0, 137</t>
   </si>
   <si>
-    <t xml:space="preserve">-0.650807,0.752774,-0.125083,572.784851,-0.757515,-0.656726,-0.004944,4.020000,-0.085680,0.091420,0.993538,20.255424,0.000000,0.000000,0.000000,1.000000</t>
+    <t xml:space="preserve">0.523656,-0.852103,0.016146,40.158855,0.840651,0.519553,0.154678,-353.890869,-0.140165,-0.067421,0.987987,23.182028,0.000000,0.000000,0.000000,1.000000</t>
   </si>
   <si>
-    <t xml:space="preserve">0, 1002</t>
+    <t xml:space="preserve">0, 152</t>
   </si>
   <si>
-    <t xml:space="preserve">-0.146911,-0.984625,0.125225,4.781213,0.990658,-0.152018,-0.028698,-189.964249,0.047178,0.119658,0.993249,19.294014,0.000000,0.000000,0.000000,1.000000</t>
+    <t xml:space="preserve">0.039280,-0.994418,-0.101220,228.471268,0.996181,0.030650,0.085366,-326.764984,-0.081766,-0.104177,0.991378,9.133189,0.000000,0.000000,0.000000,1.000000</t>
   </si>
 </sst>
 </file>
@@ -425,7 +425,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -445,7 +445,7 @@
               <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
                 <a:latin typeface="Arial"/>
               </a:rPr>
-              <a:t>Rotation X Over Time</a:t>
+              <a:t>Rotation X Over Time (radians in terms of pi)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -490,37 +490,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>1.07624694513557</c:v>
+                  <c:v>0.342580042611756</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.944587941366814</c:v>
+                  <c:v>0.594553798255268</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.14504890184726</c:v>
+                  <c:v>0.441611205637857</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.23994618256158</c:v>
+                  <c:v>0.350489225446861</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.17816008461766</c:v>
+                  <c:v>0.346946046585263</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.903675841895296</c:v>
+                  <c:v>0.411724527044866</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.945509495283548</c:v>
+                  <c:v>0.314481616521338</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.08498249069597</c:v>
+                  <c:v>0.352330418782896</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.3691791058195</c:v>
+                  <c:v>0.304587426693744</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.43396060208831</c:v>
+                  <c:v>0.381010879923099</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.68250494040814</c:v>
+                  <c:v>0.4322064473861</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -535,11 +535,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="44832367"/>
-        <c:axId val="85181980"/>
+        <c:axId val="71916666"/>
+        <c:axId val="6977623"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="44832367"/>
+        <c:axId val="71916666"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -576,14 +576,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="85181980"/>
+        <c:crossAx val="6977623"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="85181980"/>
+        <c:axId val="6977623"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -620,7 +620,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="44832367"/>
+        <c:crossAx val="71916666"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -647,7 +647,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -667,7 +667,229 @@
               <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
                 <a:latin typeface="Arial"/>
               </a:rPr>
-              <a:t>Rotation Y Over Time</a:t>
+              <a:t>Error Over Time (mm)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$W$4,Sheet1!$W$9,Sheet1!$W$14,Sheet1!$W$19,Sheet1!$W$24,Sheet1!$W$29,Sheet1!$W$34,Sheet1!$W$39,Sheet1!$W$44,Sheet1!$W$49,Sheet1!$W$54</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>13.740281</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14.190931</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12.486429</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13.750201</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16.767817</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>18.100413</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>16.334937</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>15.738484</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>19.273281</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>14.841331</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12.612013</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:hiLowLines>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:hiLowLines>
+        <c:marker val="0"/>
+        <c:axId val="56339013"/>
+        <c:axId val="3825091"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="56339013"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="3825091"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="3825091"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="56339013"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>Rotation Y Over Time (radians in terms of pi)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -712,37 +934,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.905897099195193</c:v>
+                  <c:v>0.288356002539048</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.05097536152061</c:v>
+                  <c:v>0.580924121668028</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.23169640252914</c:v>
+                  <c:v>0.518333689353279</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.41665312152141</c:v>
+                  <c:v>0.359326741761987</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.17896289591019</c:v>
+                  <c:v>0.358533836217367</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.0307280825386</c:v>
+                  <c:v>0.390056530147131</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.07988134912325</c:v>
+                  <c:v>0.341965191360336</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.09866485704261</c:v>
+                  <c:v>0.34711508311304</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.21632384883401</c:v>
+                  <c:v>0.407629011756297</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.30214184943309</c:v>
+                  <c:v>0.500453250450588</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.61293616911714</c:v>
+                  <c:v>0.486184485935403</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -757,11 +979,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="35302369"/>
-        <c:axId val="95463209"/>
+        <c:axId val="52612342"/>
+        <c:axId val="44206142"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="35302369"/>
+        <c:axId val="52612342"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -798,14 +1020,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="95463209"/>
+        <c:crossAx val="44206142"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="95463209"/>
+        <c:axId val="44206142"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -842,7 +1064,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="35302369"/>
+        <c:crossAx val="52612342"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -869,7 +1091,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -889,7 +1111,7 @@
               <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
                 <a:latin typeface="Arial"/>
               </a:rPr>
-              <a:t>Rotation Z Over Time</a:t>
+              <a:t>Rotation Z Over Time (radians in terms of pi)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -934,37 +1156,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>1.17283861599452</c:v>
+                  <c:v>0.373326126369171</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.26512910509814</c:v>
+                  <c:v>0.107518382804691</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.26291668420554</c:v>
+                  <c:v>0.102092599567219</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.00580113672097</c:v>
+                  <c:v>0.552742697925018</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.19252161546665</c:v>
+                  <c:v>0.531166733691269</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.614173174677072</c:v>
+                  <c:v>0.0786695481736275</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.03863983587122</c:v>
+                  <c:v>0.564679095448914</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.5584093952175</c:v>
+                  <c:v>0.188851464064189</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.223601057121948</c:v>
+                  <c:v>0.757363381421114</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.216806550373813</c:v>
+                  <c:v>1.02870821036555</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3.64714701659245</c:v>
+                  <c:v>1.17029886855501</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -979,11 +1201,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="31877396"/>
-        <c:axId val="70944020"/>
+        <c:axId val="39609980"/>
+        <c:axId val="99959336"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="31877396"/>
+        <c:axId val="39609980"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1020,14 +1242,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="70944020"/>
+        <c:crossAx val="99959336"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="70944020"/>
+        <c:axId val="99959336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1064,7 +1286,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="31877396"/>
+        <c:crossAx val="39609980"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1091,7 +1313,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1111,7 +1333,7 @@
               <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
                 <a:latin typeface="Arial"/>
               </a:rPr>
-              <a:t>Translation X Over Time</a:t>
+              <a:t>Translation X Over Time (mm)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1159,34 +1381,34 @@
                   <c:v>105.507744</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>17.291636</c:v>
+                  <c:v>365.957153</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>113.360664</c:v>
+                  <c:v>165.083847</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>36.035782</c:v>
+                  <c:v>377.185303</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>277.117615</c:v>
+                  <c:v>418.824707</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>80.513031</c:v>
+                  <c:v>483.649475</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.415299</c:v>
+                  <c:v>28.411476</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>406.981018</c:v>
+                  <c:v>51.365917</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>541.121033</c:v>
+                  <c:v>-4.25608</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>572.784851</c:v>
+                  <c:v>40.158855</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4.781213</c:v>
+                  <c:v>228.471268</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1201,11 +1423,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="6992357"/>
-        <c:axId val="58984280"/>
+        <c:axId val="27213662"/>
+        <c:axId val="59475455"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="6992357"/>
+        <c:axId val="27213662"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1242,14 +1464,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="58984280"/>
+        <c:crossAx val="59475455"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="58984280"/>
+        <c:axId val="59475455"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1277,7 +1499,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="6992357"/>
+        <c:crossAx val="27213662"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1304,7 +1526,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1324,7 +1546,7 @@
               <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
                 <a:latin typeface="Arial"/>
               </a:rPr>
-              <a:t>Translation Y Over Time</a:t>
+              <a:t>Translation Y Over Time (mm)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1372,34 +1594,34 @@
                   <c:v>-5.961123</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-101.650093</c:v>
+                  <c:v>464.012634</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>87.048065</c:v>
+                  <c:v>86.358902</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-247.709656</c:v>
+                  <c:v>-272.454346</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-243.577972</c:v>
+                  <c:v>-275.484131</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-55.344742</c:v>
+                  <c:v>-113.468079</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-50.014515</c:v>
+                  <c:v>-135.075256</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-207.154755</c:v>
+                  <c:v>37.332489</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-150.694366</c:v>
+                  <c:v>-313.379272</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4.02</c:v>
+                  <c:v>-353.890869</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-189.964249</c:v>
+                  <c:v>-326.764984</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1414,11 +1636,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="30801151"/>
-        <c:axId val="8821160"/>
+        <c:axId val="80929511"/>
+        <c:axId val="4327842"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="30801151"/>
+        <c:axId val="80929511"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1455,14 +1677,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="8821160"/>
+        <c:crossAx val="4327842"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="8821160"/>
+        <c:axId val="4327842"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1499,7 +1721,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="30801151"/>
+        <c:crossAx val="80929511"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1526,7 +1748,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1546,7 +1768,7 @@
               <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
                 <a:latin typeface="Arial"/>
               </a:rPr>
-              <a:t>Translation Z Over Time</a:t>
+              <a:t>Translation Z Over Time (mm)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1594,34 +1816,34 @@
                   <c:v>-3.172411</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-4.618966</c:v>
+                  <c:v>65.647797</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-7.875946</c:v>
+                  <c:v>-10.808743</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>11.49333</c:v>
+                  <c:v>9.64325</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-0.079196</c:v>
+                  <c:v>15.78432</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-10.107821</c:v>
+                  <c:v>13.690338</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-5.052285</c:v>
+                  <c:v>-3.179838</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.413674</c:v>
+                  <c:v>-0.523544</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>23.79402</c:v>
+                  <c:v>9.232149</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>20.255424</c:v>
+                  <c:v>23.182028</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>19.294014</c:v>
+                  <c:v>9.133189</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1636,11 +1858,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="55166715"/>
-        <c:axId val="45438906"/>
+        <c:axId val="88132280"/>
+        <c:axId val="99128794"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="55166715"/>
+        <c:axId val="88132280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1677,14 +1899,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="45438906"/>
+        <c:crossAx val="99128794"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="45438906"/>
+        <c:axId val="99128794"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1721,7 +1943,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="55166715"/>
+        <c:crossAx val="88132280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1748,7 +1970,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1816,34 +2038,34 @@
                   <c:v>0.994861</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.996163</c:v>
+                  <c:v>0.038663</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.798334</c:v>
+                  <c:v>0.035316</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.635223</c:v>
+                  <c:v>-0.95378</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-0.879993</c:v>
+                  <c:v>-0.959883</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.963433</c:v>
+                  <c:v>-0.769638</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.001365</c:v>
+                  <c:v>0.950592</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-0.974733</c:v>
+                  <c:v>0.960013</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-0.692475</c:v>
+                  <c:v>0.838037</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-0.650807</c:v>
+                  <c:v>0.523656</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-0.146911</c:v>
+                  <c:v>0.03928</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1858,11 +2080,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="4442823"/>
-        <c:axId val="97676177"/>
+        <c:axId val="81845336"/>
+        <c:axId val="90300955"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="4442823"/>
+        <c:axId val="81845336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1899,14 +2121,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="97676177"/>
+        <c:crossAx val="90300955"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="97676177"/>
+        <c:axId val="90300955"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1943,7 +2165,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="4442823"/>
+        <c:crossAx val="81845336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1970,7 +2192,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2038,34 +2260,34 @@
                   <c:v>0.999039</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.993708</c:v>
+                  <c:v>0.032822</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.797144</c:v>
+                  <c:v>0.030794</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.634262</c:v>
+                  <c:v>-0.955319</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-0.88026</c:v>
+                  <c:v>-0.963655</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.958717</c:v>
+                  <c:v>-0.769464</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.999511</c:v>
+                  <c:v>0.948474</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-0.977623</c:v>
+                  <c:v>0.960046</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-0.686231</c:v>
+                  <c:v>0.828682</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-0.656726</c:v>
+                  <c:v>0.519553</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-0.152018</c:v>
+                  <c:v>0.03065</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2080,11 +2302,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="86278976"/>
-        <c:axId val="75981070"/>
+        <c:axId val="92357916"/>
+        <c:axId val="34162294"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="86278976"/>
+        <c:axId val="92357916"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2121,14 +2343,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="75981070"/>
+        <c:crossAx val="34162294"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="75981070"/>
+        <c:axId val="34162294"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2165,7 +2387,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="86278976"/>
+        <c:crossAx val="92357916"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2192,7 +2414,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2260,34 +2482,34 @@
                   <c:v>0.995803</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.997369</c:v>
+                  <c:v>0.961686</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.998988</c:v>
+                  <c:v>0.992215</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.997901</c:v>
+                  <c:v>0.997762</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.000556</c:v>
+                  <c:v>0.995269</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.99382</c:v>
+                  <c:v>0.997565</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.998602</c:v>
+                  <c:v>0.99736</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.998395</c:v>
+                  <c:v>1.000038</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.990955</c:v>
+                  <c:v>0.989705</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.993538</c:v>
+                  <c:v>0.987987</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.993249</c:v>
+                  <c:v>0.991378</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2302,11 +2524,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="1027763"/>
-        <c:axId val="31319659"/>
+        <c:axId val="65151711"/>
+        <c:axId val="18825537"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1027763"/>
+        <c:axId val="65151711"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2343,14 +2565,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="31319659"/>
+        <c:crossAx val="18825537"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="31319659"/>
+        <c:axId val="18825537"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2387,229 +2609,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1027763"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:solidFill>
-            <a:srgbClr val="b3b3b3"/>
-          </a:solidFill>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="ffffff"/>
-    </a:solidFill>
-    <a:ln>
-      <a:noFill/>
-    </a:ln>
-  </c:spPr>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart20.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
-                <a:latin typeface="Arial"/>
-              </a:rPr>
-              <a:t>Error Over Time</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="004586"/>
-            </a:solidFill>
-            <a:ln w="28800">
-              <a:solidFill>
-                <a:srgbClr val="004586"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:dLbls>
-            <c:numFmt formatCode="General" sourceLinked="1"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$W$4,Sheet1!$W$9,Sheet1!$W$14,Sheet1!$W$19,Sheet1!$W$24,Sheet1!$W$29,Sheet1!$W$34,Sheet1!$W$39,Sheet1!$W$44,Sheet1!$W$49,Sheet1!$W$54</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>13.740281</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>15.816349</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>17.676696</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>14.589707</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>15.88971</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>16.041497</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>9.341261</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>16.438241</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>17.81745</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>20.711356</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>17.666445</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:hiLowLines>
-          <c:spPr>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:hiLowLines>
-        <c:marker val="0"/>
-        <c:axId val="93860734"/>
-        <c:axId val="48616619"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="93860734"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="b3b3b3"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln>
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="48616619"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="48616619"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="b3b3b3"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln>
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="93860734"/>
+        <c:crossAx val="65151711"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2670,16 +2670,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>6840</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>-360</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>809640</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>9360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>31</xdr:col>
-      <xdr:colOff>72720</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>153000</xdr:rowOff>
+      <xdr:colOff>62640</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>162360</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2687,7 +2687,7 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="28282680" y="3900960"/>
+        <a:off x="28272600" y="4073040"/>
         <a:ext cx="5755320" cy="3241800"/>
       </xdr:xfrm>
       <a:graphic>
@@ -2701,15 +2701,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>779400</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>153360</xdr:rowOff>
+      <xdr:colOff>808920</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>19080</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>31</xdr:col>
-      <xdr:colOff>42120</xdr:colOff>
-      <xdr:row>64</xdr:row>
-      <xdr:rowOff>144000</xdr:rowOff>
+      <xdr:colOff>71640</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>9720</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2717,7 +2717,7 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="28242360" y="7305840"/>
+        <a:off x="28271880" y="7659360"/>
         <a:ext cx="5765040" cy="3241800"/>
       </xdr:xfrm>
       <a:graphic>
@@ -2949,7 +2949,7 @@
   <dimension ref="B2:W57"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="topLeft" activeCell="AY31" activeCellId="0" sqref="AY31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3020,39 +3020,39 @@
         <v>105.507744</v>
       </c>
       <c r="K4" s="0" t="n">
-        <f aca="false">COS(G5) - SIN(H5) + SIN(G6) + COS(H6)</f>
-        <v>1.07624694513557</v>
+        <f aca="false"> (COS(G5) - SIN(H5) + SIN(G6) + COS(H6)) / PI()</f>
+        <v>0.342580042611756</v>
       </c>
       <c r="L4" s="0" t="n">
-        <f aca="false">COS(F4) + SIN(H4) - SIN(F6) + COS(H6)</f>
-        <v>0.905897099195193</v>
+        <f aca="false"> (COS(F4) + SIN(H4) - SIN(F6) + COS(H6)) / PI()</f>
+        <v>0.288356002539048</v>
       </c>
       <c r="M4" s="0" t="n">
-        <f aca="false">COS(F4) - SIN(G4) + SIN(F5) + COS(G5)</f>
-        <v>1.17283861599452</v>
+        <f aca="false"> (COS(F4) - SIN(G4) + SIN(F5) + COS(G5)) / PI()</f>
+        <v>0.373326126369171</v>
       </c>
       <c r="O4" s="0" t="n">
-        <f aca="false">I4</f>
+        <f aca="false"> I4</f>
         <v>105.507744</v>
       </c>
       <c r="P4" s="0" t="n">
-        <f aca="false">I5</f>
+        <f aca="false"> I5</f>
         <v>-5.961123</v>
       </c>
       <c r="Q4" s="0" t="n">
-        <f aca="false">I6</f>
+        <f aca="false"> I6</f>
         <v>-3.172411</v>
       </c>
       <c r="S4" s="0" t="n">
-        <f aca="false">F4</f>
+        <f aca="false"> F4</f>
         <v>0.994861</v>
       </c>
       <c r="T4" s="0" t="n">
-        <f aca="false">G5</f>
+        <f aca="false"> G5</f>
         <v>0.999039</v>
       </c>
       <c r="U4" s="0" t="n">
-        <f aca="false">H6</f>
+        <f aca="false"> H6</f>
         <v>0.995803</v>
       </c>
       <c r="W4" s="0" t="n">
@@ -3109,83 +3109,83 @@
         <v>16</v>
       </c>
       <c r="F9" s="0" t="n">
-        <v>0.996163</v>
+        <v>0.038663</v>
       </c>
       <c r="G9" s="0" t="n">
-        <v>-0.087481</v>
+        <v>0.999155</v>
       </c>
       <c r="H9" s="0" t="n">
-        <v>-0.020706</v>
+        <v>-0.015959</v>
       </c>
       <c r="I9" s="0" t="n">
-        <v>17.291636</v>
+        <v>365.957153</v>
       </c>
       <c r="K9" s="0" t="n">
-        <f aca="false">COS(G10) - SIN(H10) + SIN(G11) + COS(H11)</f>
-        <v>0.944587941366814</v>
+        <f aca="false"> (COS(G10) - SIN(H10) + SIN(G11) + COS(H11)) / PI()</f>
+        <v>0.594553798255268</v>
       </c>
       <c r="L9" s="0" t="n">
-        <f aca="false">COS(F9) + SIN(H9) - SIN(F11) + COS(H11)</f>
-        <v>1.05097536152061</v>
+        <f aca="false"> (COS(F9) + SIN(H9) - SIN(F11) + COS(H11)) / PI()</f>
+        <v>0.580924121668028</v>
       </c>
       <c r="M9" s="0" t="n">
-        <f aca="false">COS(F9) - SIN(G9) + SIN(F10) + COS(G10)</f>
-        <v>1.26512910509814</v>
+        <f aca="false"> (COS(F9) - SIN(G9) + SIN(F10) + COS(G10)) / PI()</f>
+        <v>0.107518382804691</v>
       </c>
       <c r="O9" s="0" t="n">
-        <f aca="false">I9</f>
-        <v>17.291636</v>
+        <f aca="false"> I9</f>
+        <v>365.957153</v>
       </c>
       <c r="P9" s="0" t="n">
-        <f aca="false">I10</f>
-        <v>-101.650093</v>
+        <f aca="false"> I10</f>
+        <v>464.012634</v>
       </c>
       <c r="Q9" s="0" t="n">
-        <f aca="false">I11</f>
-        <v>-4.618966</v>
+        <f aca="false"> I11</f>
+        <v>65.647797</v>
       </c>
       <c r="S9" s="0" t="n">
-        <f aca="false">F9</f>
-        <v>0.996163</v>
+        <f aca="false"> F9</f>
+        <v>0.038663</v>
       </c>
       <c r="T9" s="0" t="n">
-        <f aca="false">G10</f>
-        <v>0.993708</v>
+        <f aca="false"> G10</f>
+        <v>0.032822</v>
       </c>
       <c r="U9" s="0" t="n">
-        <f aca="false">H11</f>
-        <v>0.997369</v>
+        <f aca="false"> H11</f>
+        <v>0.961686</v>
       </c>
       <c r="W9" s="0" t="n">
-        <v>15.816349</v>
+        <v>14.190931</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F10" s="0" t="n">
-        <v>0.088763</v>
+        <v>-0.961273</v>
       </c>
       <c r="G10" s="0" t="n">
-        <v>0.993708</v>
+        <v>0.032822</v>
       </c>
       <c r="H10" s="0" t="n">
-        <v>0.071039</v>
+        <v>-0.273733</v>
       </c>
       <c r="I10" s="0" t="n">
-        <v>-101.650093</v>
+        <v>464.012634</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F11" s="0" t="n">
-        <v>0.014362</v>
+        <v>-0.272972</v>
       </c>
       <c r="G11" s="0" t="n">
-        <v>-0.072597</v>
+        <v>0.025922</v>
       </c>
       <c r="H11" s="0" t="n">
-        <v>0.997369</v>
+        <v>0.961686</v>
       </c>
       <c r="I11" s="0" t="n">
-        <v>-4.618966</v>
+        <v>65.647797</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3210,83 +3210,83 @@
         <v>18</v>
       </c>
       <c r="F14" s="0" t="n">
-        <v>0.798334</v>
+        <v>0.035316</v>
       </c>
       <c r="G14" s="0" t="n">
-        <v>0.602807</v>
+        <v>0.992411</v>
       </c>
       <c r="H14" s="0" t="n">
-        <v>0.012228</v>
+        <v>0.118269</v>
       </c>
       <c r="I14" s="0" t="n">
-        <v>113.360664</v>
+        <v>165.083847</v>
       </c>
       <c r="K14" s="0" t="n">
-        <f aca="false">COS(G15) - SIN(H15) + SIN(G16) + COS(H16)</f>
-        <v>1.14504890184726</v>
+        <f aca="false"> (COS(G15) - SIN(H15) + SIN(G16) + COS(H16)) / PI()</f>
+        <v>0.441611205637857</v>
       </c>
       <c r="L14" s="0" t="n">
-        <f aca="false">COS(F14) + SIN(H14) - SIN(F16) + COS(H16)</f>
-        <v>1.23169640252914</v>
+        <f aca="false"> (COS(F14) + SIN(H14) - SIN(F16) + COS(H16)) / PI()</f>
+        <v>0.518333689353279</v>
       </c>
       <c r="M14" s="0" t="n">
-        <f aca="false">COS(F14) - SIN(G14) + SIN(F15) + COS(G15)</f>
-        <v>0.26291668420554</v>
+        <f aca="false"> (COS(F14) - SIN(G14) + SIN(F15) + COS(G15)) / PI()</f>
+        <v>0.102092599567219</v>
       </c>
       <c r="O14" s="0" t="n">
-        <f aca="false">I14</f>
-        <v>113.360664</v>
+        <f aca="false"> I14</f>
+        <v>165.083847</v>
       </c>
       <c r="P14" s="0" t="n">
-        <f aca="false">I15</f>
-        <v>87.048065</v>
+        <f aca="false"> I15</f>
+        <v>86.358902</v>
       </c>
       <c r="Q14" s="0" t="n">
-        <f aca="false">I16</f>
-        <v>-7.875946</v>
+        <f aca="false"> I16</f>
+        <v>-10.808743</v>
       </c>
       <c r="S14" s="0" t="n">
-        <f aca="false">F14</f>
-        <v>0.798334</v>
+        <f aca="false"> F14</f>
+        <v>0.035316</v>
       </c>
       <c r="T14" s="0" t="n">
-        <f aca="false">G15</f>
-        <v>0.797144</v>
+        <f aca="false"> G15</f>
+        <v>0.030794</v>
       </c>
       <c r="U14" s="0" t="n">
-        <f aca="false">H16</f>
-        <v>0.998988</v>
+        <f aca="false"> H16</f>
+        <v>0.992215</v>
       </c>
       <c r="W14" s="0" t="n">
-        <v>17.676696</v>
+        <v>12.486429</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F15" s="0" t="n">
-        <v>-0.602592</v>
+        <v>-0.998801</v>
       </c>
       <c r="G15" s="0" t="n">
-        <v>0.797144</v>
+        <v>0.030794</v>
       </c>
       <c r="H15" s="0" t="n">
-        <v>0.048667</v>
+        <v>0.039766</v>
       </c>
       <c r="I15" s="0" t="n">
-        <v>87.048065</v>
+        <v>86.358902</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F16" s="0" t="n">
-        <v>0.019587</v>
+        <v>0.035821</v>
       </c>
       <c r="G16" s="0" t="n">
-        <v>-0.046226</v>
+        <v>-0.119529</v>
       </c>
       <c r="H16" s="0" t="n">
-        <v>0.998988</v>
+        <v>0.992215</v>
       </c>
       <c r="I16" s="0" t="n">
-        <v>-7.875946</v>
+        <v>-10.808743</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3311,83 +3311,83 @@
         <v>20</v>
       </c>
       <c r="F19" s="0" t="n">
-        <v>0.635223</v>
+        <v>-0.95378</v>
       </c>
       <c r="G19" s="0" t="n">
-        <v>-0.773382</v>
+        <v>-0.295352</v>
       </c>
       <c r="H19" s="0" t="n">
-        <v>0.009403</v>
+        <v>-0.057124</v>
       </c>
       <c r="I19" s="0" t="n">
-        <v>36.035782</v>
+        <v>377.185303</v>
       </c>
       <c r="K19" s="0" t="n">
-        <f aca="false">COS(G20) - SIN(H20) + SIN(G21) + COS(H21)</f>
-        <v>1.23994618256158</v>
+        <f aca="false"> (COS(G20) - SIN(H20) + SIN(G21) + COS(H21)) / PI()</f>
+        <v>0.350489225446861</v>
       </c>
       <c r="L19" s="0" t="n">
-        <f aca="false">COS(F19) + SIN(H19) - SIN(F21) + COS(H21)</f>
-        <v>1.41665312152141</v>
+        <f aca="false"> (COS(F19) + SIN(H19) - SIN(F21) + COS(H21)) / PI()</f>
+        <v>0.359326741761987</v>
       </c>
       <c r="M19" s="0" t="n">
-        <f aca="false">COS(F19) - SIN(G19) + SIN(F20) + COS(G20)</f>
-        <v>3.00580113672097</v>
+        <f aca="false"> (COS(F19) - SIN(G19) + SIN(F20) + COS(G20)) / PI()</f>
+        <v>0.552742697925018</v>
       </c>
       <c r="O19" s="0" t="n">
-        <f aca="false">I19</f>
-        <v>36.035782</v>
+        <f aca="false"> I19</f>
+        <v>377.185303</v>
       </c>
       <c r="P19" s="0" t="n">
-        <f aca="false">I20</f>
-        <v>-247.709656</v>
+        <f aca="false"> I20</f>
+        <v>-272.454346</v>
       </c>
       <c r="Q19" s="0" t="n">
-        <f aca="false">I21</f>
-        <v>11.49333</v>
+        <f aca="false"> I21</f>
+        <v>9.64325</v>
       </c>
       <c r="S19" s="0" t="n">
-        <f aca="false">F19</f>
-        <v>0.635223</v>
+        <f aca="false"> F19</f>
+        <v>-0.95378</v>
       </c>
       <c r="T19" s="0" t="n">
-        <f aca="false">G20</f>
-        <v>0.634262</v>
+        <f aca="false"> G20</f>
+        <v>-0.955319</v>
       </c>
       <c r="U19" s="0" t="n">
-        <f aca="false">H21</f>
-        <v>0.997901</v>
+        <f aca="false"> H21</f>
+        <v>0.997762</v>
       </c>
       <c r="W19" s="0" t="n">
-        <v>14.589707</v>
+        <v>13.750201</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F20" s="0" t="n">
-        <v>0.770917</v>
+        <v>0.293666</v>
       </c>
       <c r="G20" s="0" t="n">
-        <v>0.634262</v>
+        <v>-0.955319</v>
       </c>
       <c r="H20" s="0" t="n">
-        <v>0.070284</v>
+        <v>0.036029</v>
       </c>
       <c r="I20" s="0" t="n">
-        <v>-247.709656</v>
+        <v>-272.454346</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F21" s="0" t="n">
-        <v>-0.06028</v>
+        <v>-0.065209</v>
       </c>
       <c r="G21" s="0" t="n">
-        <v>-0.037413</v>
+        <v>0.017584</v>
       </c>
       <c r="H21" s="0" t="n">
-        <v>0.997901</v>
+        <v>0.997762</v>
       </c>
       <c r="I21" s="0" t="n">
-        <v>11.49333</v>
+        <v>9.64325</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3412,83 +3412,83 @@
         <v>22</v>
       </c>
       <c r="F24" s="0" t="n">
-        <v>-0.879993</v>
+        <v>-0.959883</v>
       </c>
       <c r="G24" s="0" t="n">
-        <v>-0.477127</v>
+        <v>-0.266864</v>
       </c>
       <c r="H24" s="0" t="n">
-        <v>0.003769</v>
+        <v>-0.087477</v>
       </c>
       <c r="I24" s="0" t="n">
-        <v>277.117615</v>
+        <v>418.824707</v>
       </c>
       <c r="K24" s="0" t="n">
-        <f aca="false">COS(G25) - SIN(H25) + SIN(G26) + COS(H26)</f>
-        <v>1.17816008461766</v>
+        <f aca="false"> (COS(G25) - SIN(H25) + SIN(G26) + COS(H26)) / PI()</f>
+        <v>0.346946046585263</v>
       </c>
       <c r="L24" s="0" t="n">
-        <f aca="false">COS(F24) + SIN(H24) - SIN(F26) + COS(H26)</f>
-        <v>1.17896289591019</v>
+        <f aca="false"> (COS(F24) + SIN(H24) - SIN(F26) + COS(H26)) / PI()</f>
+        <v>0.358533836217367</v>
       </c>
       <c r="M24" s="0" t="n">
-        <f aca="false">COS(F24) - SIN(G24) + SIN(F25) + COS(G25)</f>
-        <v>2.19252161546665</v>
+        <f aca="false"> (COS(F24) - SIN(G24) + SIN(F25) + COS(G25)) / PI()</f>
+        <v>0.531166733691269</v>
       </c>
       <c r="O24" s="0" t="n">
-        <f aca="false">I24</f>
-        <v>277.117615</v>
+        <f aca="false"> I24</f>
+        <v>418.824707</v>
       </c>
       <c r="P24" s="0" t="n">
-        <f aca="false">I25</f>
-        <v>-243.577972</v>
+        <f aca="false"> I25</f>
+        <v>-275.484131</v>
       </c>
       <c r="Q24" s="0" t="n">
-        <f aca="false">I26</f>
-        <v>-0.079196</v>
+        <f aca="false"> I26</f>
+        <v>15.78432</v>
       </c>
       <c r="S24" s="0" t="n">
-        <f aca="false">F24</f>
-        <v>-0.879993</v>
+        <f aca="false"> F24</f>
+        <v>-0.959883</v>
       </c>
       <c r="T24" s="0" t="n">
-        <f aca="false">G25</f>
-        <v>-0.88026</v>
+        <f aca="false"> G25</f>
+        <v>-0.963655</v>
       </c>
       <c r="U24" s="0" t="n">
-        <f aca="false">H26</f>
-        <v>1.000556</v>
+        <f aca="false"> H26</f>
+        <v>0.995269</v>
       </c>
       <c r="W24" s="0" t="n">
-        <v>15.88971</v>
+        <v>16.767817</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F25" s="0" t="n">
-        <v>0.477078</v>
+        <v>0.263917</v>
       </c>
       <c r="G25" s="0" t="n">
-        <v>-0.88026</v>
+        <v>-0.963655</v>
       </c>
       <c r="H25" s="0" t="n">
-        <v>0.003191</v>
+        <v>0.043828</v>
       </c>
       <c r="I25" s="0" t="n">
-        <v>-243.577972</v>
+        <v>-275.484131</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F26" s="0" t="n">
-        <v>0.001797</v>
+        <v>-0.095987</v>
       </c>
       <c r="G26" s="0" t="n">
-        <v>0.004566</v>
+        <v>0.018979</v>
       </c>
       <c r="H26" s="0" t="n">
-        <v>1.000556</v>
+        <v>0.995269</v>
       </c>
       <c r="I26" s="0" t="n">
-        <v>-0.079196</v>
+        <v>15.78432</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3513,83 +3513,83 @@
         <v>24</v>
       </c>
       <c r="F29" s="0" t="n">
-        <v>0.963433</v>
+        <v>-0.769638</v>
       </c>
       <c r="G29" s="0" t="n">
-        <v>0.271132</v>
+        <v>0.63556</v>
       </c>
       <c r="H29" s="0" t="n">
-        <v>-0.02787</v>
+        <v>-0.063222</v>
       </c>
       <c r="I29" s="0" t="n">
-        <v>80.513031</v>
+        <v>483.649475</v>
       </c>
       <c r="K29" s="0" t="n">
-        <f aca="false">COS(G30) - SIN(H30) + SIN(G31) + COS(H31)</f>
-        <v>0.903675841895296</v>
+        <f aca="false"> (COS(G30) - SIN(H30) + SIN(G31) + COS(H31)) / PI()</f>
+        <v>0.411724527044866</v>
       </c>
       <c r="L29" s="0" t="n">
-        <f aca="false">COS(F29) + SIN(H29) - SIN(F31) + COS(H31)</f>
-        <v>1.0307280825386</v>
+        <f aca="false"> (COS(F29) + SIN(H29) - SIN(F31) + COS(H31)) / PI()</f>
+        <v>0.390056530147131</v>
       </c>
       <c r="M29" s="0" t="n">
-        <f aca="false">COS(F29) - SIN(G29) + SIN(F30) + COS(G30)</f>
-        <v>0.614173174677072</v>
+        <f aca="false"> (COS(F29) - SIN(G29) + SIN(F30) + COS(G30)) / PI()</f>
+        <v>0.0786695481736275</v>
       </c>
       <c r="O29" s="0" t="n">
-        <f aca="false">I29</f>
-        <v>80.513031</v>
+        <f aca="false"> I29</f>
+        <v>483.649475</v>
       </c>
       <c r="P29" s="0" t="n">
-        <f aca="false">I30</f>
-        <v>-55.344742</v>
+        <f aca="false"> I30</f>
+        <v>-113.468079</v>
       </c>
       <c r="Q29" s="0" t="n">
-        <f aca="false">I31</f>
-        <v>-10.107821</v>
+        <f aca="false"> I31</f>
+        <v>13.690338</v>
       </c>
       <c r="S29" s="0" t="n">
-        <f aca="false">F29</f>
-        <v>0.963433</v>
+        <f aca="false"> F29</f>
+        <v>-0.769638</v>
       </c>
       <c r="T29" s="0" t="n">
-        <f aca="false">G30</f>
-        <v>0.958717</v>
+        <f aca="false"> G30</f>
+        <v>-0.769464</v>
       </c>
       <c r="U29" s="0" t="n">
-        <f aca="false">H31</f>
-        <v>0.99382</v>
+        <f aca="false"> H31</f>
+        <v>0.997565</v>
       </c>
       <c r="W29" s="0" t="n">
-        <v>16.041497</v>
+        <v>18.100413</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F30" s="0" t="n">
-        <v>-0.26642</v>
+        <v>-0.6381</v>
       </c>
       <c r="G30" s="0" t="n">
-        <v>0.958717</v>
+        <v>-0.769464</v>
       </c>
       <c r="H30" s="0" t="n">
-        <v>0.114203</v>
+        <v>0.032367</v>
       </c>
       <c r="I30" s="0" t="n">
-        <v>-55.344742</v>
+        <v>-113.468079</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F31" s="0" t="n">
-        <v>0.057634</v>
+        <v>-0.02807</v>
       </c>
       <c r="G31" s="0" t="n">
-        <v>-0.102612</v>
+        <v>0.065245</v>
       </c>
       <c r="H31" s="0" t="n">
-        <v>0.99382</v>
+        <v>0.997565</v>
       </c>
       <c r="I31" s="0" t="n">
-        <v>-10.107821</v>
+        <v>13.690338</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3614,83 +3614,83 @@
         <v>26</v>
       </c>
       <c r="F34" s="0" t="n">
-        <v>1.001365</v>
+        <v>0.950592</v>
       </c>
       <c r="G34" s="0" t="n">
-        <v>0.020552</v>
+        <v>-0.30899</v>
       </c>
       <c r="H34" s="0" t="n">
-        <v>0.000337</v>
+        <v>-0.035646</v>
       </c>
       <c r="I34" s="0" t="n">
-        <v>2.415299</v>
+        <v>28.411476</v>
       </c>
       <c r="K34" s="0" t="n">
-        <f aca="false">COS(G35) - SIN(H35) + SIN(G36) + COS(H36)</f>
-        <v>0.945509495283548</v>
+        <f aca="false"> (COS(G35) - SIN(H35) + SIN(G36) + COS(H36)) / PI()</f>
+        <v>0.314481616521338</v>
       </c>
       <c r="L34" s="0" t="n">
-        <f aca="false">COS(F34) + SIN(H34) - SIN(F36) + COS(H36)</f>
-        <v>1.07988134912325</v>
+        <f aca="false"> (COS(F34) + SIN(H34) - SIN(F36) + COS(H36)) / PI()</f>
+        <v>0.341965191360336</v>
       </c>
       <c r="M34" s="0" t="n">
-        <f aca="false">COS(F34) - SIN(G34) + SIN(F35) + COS(G35)</f>
-        <v>1.03863983587122</v>
+        <f aca="false"> (COS(F34) - SIN(G34) + SIN(F35) + COS(G35)) / PI()</f>
+        <v>0.564679095448914</v>
       </c>
       <c r="O34" s="0" t="n">
-        <f aca="false">I34</f>
-        <v>2.415299</v>
+        <f aca="false"> I34</f>
+        <v>28.411476</v>
       </c>
       <c r="P34" s="0" t="n">
-        <f aca="false">I35</f>
-        <v>-50.014515</v>
+        <f aca="false"> I35</f>
+        <v>-135.075256</v>
       </c>
       <c r="Q34" s="0" t="n">
-        <f aca="false">I36</f>
-        <v>-5.052285</v>
+        <f aca="false"> I36</f>
+        <v>-3.179838</v>
       </c>
       <c r="S34" s="0" t="n">
-        <f aca="false">F34</f>
-        <v>1.001365</v>
+        <f aca="false"> F34</f>
+        <v>0.950592</v>
       </c>
       <c r="T34" s="0" t="n">
-        <f aca="false">G35</f>
-        <v>0.999511</v>
+        <f aca="false"> G35</f>
+        <v>0.948474</v>
       </c>
       <c r="U34" s="0" t="n">
-        <f aca="false">H36</f>
-        <v>0.998602</v>
+        <f aca="false"> H36</f>
+        <v>0.99736</v>
       </c>
       <c r="W34" s="0" t="n">
-        <v>9.341261</v>
+        <v>16.334937</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F35" s="0" t="n">
-        <v>-0.020678</v>
+        <v>0.310747</v>
       </c>
       <c r="G35" s="0" t="n">
-        <v>0.999511</v>
+        <v>0.948474</v>
       </c>
       <c r="H35" s="0" t="n">
-        <v>0.06833</v>
+        <v>0.064858</v>
       </c>
       <c r="I35" s="0" t="n">
-        <v>-50.014515</v>
+        <v>-135.075256</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F36" s="0" t="n">
-        <v>0.001087</v>
+        <v>0.01377</v>
       </c>
       <c r="G36" s="0" t="n">
-        <v>-0.068459</v>
+        <v>-0.072724</v>
       </c>
       <c r="H36" s="0" t="n">
-        <v>0.998602</v>
+        <v>0.99736</v>
       </c>
       <c r="I36" s="0" t="n">
-        <v>-5.052285</v>
+        <v>-3.179838</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3715,83 +3715,83 @@
         <v>28</v>
       </c>
       <c r="F39" s="0" t="n">
-        <v>-0.974733</v>
+        <v>0.960013</v>
       </c>
       <c r="G39" s="0" t="n">
-        <v>-0.220065</v>
+        <v>0.280538</v>
       </c>
       <c r="H39" s="0" t="n">
-        <v>-0.071898</v>
+        <v>-0.011149</v>
       </c>
       <c r="I39" s="0" t="n">
-        <v>406.981018</v>
+        <v>51.365917</v>
       </c>
       <c r="K39" s="0" t="n">
-        <f aca="false">COS(G40) - SIN(H40) + SIN(G41) + COS(H41)</f>
-        <v>1.08498249069597</v>
+        <f aca="false"> (COS(G40) - SIN(H40) + SIN(G41) + COS(H41)) / PI()</f>
+        <v>0.352330418782896</v>
       </c>
       <c r="L39" s="0" t="n">
-        <f aca="false">COS(F39) + SIN(H39) - SIN(F41) + COS(H41)</f>
-        <v>1.09866485704261</v>
+        <f aca="false"> (COS(F39) + SIN(H39) - SIN(F41) + COS(H41)) / PI()</f>
+        <v>0.34711508311304</v>
       </c>
       <c r="M39" s="0" t="n">
-        <f aca="false">COS(F39) - SIN(G39) + SIN(F40) + COS(G40)</f>
-        <v>1.5584093952175</v>
+        <f aca="false"> (COS(F39) - SIN(G39) + SIN(F40) + COS(G40)) / PI()</f>
+        <v>0.188851464064189</v>
       </c>
       <c r="O39" s="0" t="n">
-        <f aca="false">I39</f>
-        <v>406.981018</v>
+        <f aca="false"> I39</f>
+        <v>51.365917</v>
       </c>
       <c r="P39" s="0" t="n">
-        <f aca="false">I40</f>
-        <v>-207.154755</v>
+        <f aca="false"> I40</f>
+        <v>37.332489</v>
       </c>
       <c r="Q39" s="0" t="n">
-        <f aca="false">I41</f>
-        <v>4.413674</v>
+        <f aca="false"> I41</f>
+        <v>-0.523544</v>
       </c>
       <c r="S39" s="0" t="n">
-        <f aca="false">F39</f>
-        <v>-0.974733</v>
+        <f aca="false"> F39</f>
+        <v>0.960013</v>
       </c>
       <c r="T39" s="0" t="n">
-        <f aca="false">G40</f>
-        <v>-0.977623</v>
+        <f aca="false"> G40</f>
+        <v>0.960046</v>
       </c>
       <c r="U39" s="0" t="n">
-        <f aca="false">H41</f>
-        <v>0.998395</v>
+        <f aca="false"> H41</f>
+        <v>1.000038</v>
       </c>
       <c r="W39" s="0" t="n">
-        <v>16.438241</v>
+        <v>15.738484</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F40" s="0" t="n">
-        <v>0.22154</v>
+        <v>-0.280488</v>
       </c>
       <c r="G40" s="0" t="n">
-        <v>-0.977623</v>
+        <v>0.960046</v>
       </c>
       <c r="H40" s="0" t="n">
-        <v>-0.012048</v>
+        <v>0.005101</v>
       </c>
       <c r="I40" s="0" t="n">
-        <v>-207.154755</v>
+        <v>37.332489</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F41" s="0" t="n">
-        <v>-0.067511</v>
+        <v>0.012137</v>
       </c>
       <c r="G41" s="0" t="n">
-        <v>-0.027716</v>
+        <v>-0.001773</v>
       </c>
       <c r="H41" s="0" t="n">
-        <v>0.998395</v>
+        <v>1.000038</v>
       </c>
       <c r="I41" s="0" t="n">
-        <v>4.413674</v>
+        <v>-0.523544</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3816,83 +3816,83 @@
         <v>30</v>
       </c>
       <c r="F44" s="0" t="n">
-        <v>-0.692475</v>
+        <v>0.838037</v>
       </c>
       <c r="G44" s="0" t="n">
-        <v>0.716978</v>
+        <v>-0.545962</v>
       </c>
       <c r="H44" s="0" t="n">
-        <v>-0.106717</v>
+        <v>-0.008549</v>
       </c>
       <c r="I44" s="0" t="n">
-        <v>541.121033</v>
+        <v>-4.25608</v>
       </c>
       <c r="K44" s="0" t="n">
-        <f aca="false">COS(G45) - SIN(H45) + SIN(G46) + COS(H46)</f>
-        <v>1.3691791058195</v>
+        <f aca="false"> (COS(G45) - SIN(H45) + SIN(G46) + COS(H46)) / PI()</f>
+        <v>0.304587426693744</v>
       </c>
       <c r="L44" s="0" t="n">
-        <f aca="false">COS(F44) + SIN(H44) - SIN(F46) + COS(H46)</f>
-        <v>1.21632384883401</v>
+        <f aca="false"> (COS(F44) + SIN(H44) - SIN(F46) + COS(H46)) / PI()</f>
+        <v>0.407629011756297</v>
       </c>
       <c r="M44" s="0" t="n">
-        <f aca="false">COS(F44) - SIN(G44) + SIN(F45) + COS(G45)</f>
-        <v>0.223601057121948</v>
+        <f aca="false"> (COS(F44) - SIN(G44) + SIN(F45) + COS(G45)) / PI()</f>
+        <v>0.757363381421114</v>
       </c>
       <c r="O44" s="0" t="n">
-        <f aca="false">I44</f>
-        <v>541.121033</v>
+        <f aca="false"> I44</f>
+        <v>-4.25608</v>
       </c>
       <c r="P44" s="0" t="n">
-        <f aca="false">I45</f>
-        <v>-150.694366</v>
+        <f aca="false"> I45</f>
+        <v>-313.379272</v>
       </c>
       <c r="Q44" s="0" t="n">
-        <f aca="false">I46</f>
-        <v>23.79402</v>
+        <f aca="false"> I46</f>
+        <v>9.232149</v>
       </c>
       <c r="S44" s="0" t="n">
-        <f aca="false">F44</f>
-        <v>-0.692475</v>
+        <f aca="false"> F44</f>
+        <v>0.838037</v>
       </c>
       <c r="T44" s="0" t="n">
-        <f aca="false">G45</f>
-        <v>-0.686231</v>
+        <f aca="false"> G45</f>
+        <v>0.828682</v>
       </c>
       <c r="U44" s="0" t="n">
-        <f aca="false">H46</f>
-        <v>0.990955</v>
+        <f aca="false"> H46</f>
+        <v>0.989705</v>
       </c>
       <c r="W44" s="0" t="n">
-        <v>17.81745</v>
+        <v>19.273281</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F45" s="0" t="n">
-        <v>-0.724281</v>
+        <v>0.541376</v>
       </c>
       <c r="G45" s="0" t="n">
-        <v>-0.686231</v>
+        <v>0.828682</v>
       </c>
       <c r="H45" s="0" t="n">
-        <v>0.094788</v>
+        <v>0.143686</v>
       </c>
       <c r="I45" s="0" t="n">
-        <v>-150.694366</v>
+        <v>-313.379272</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F46" s="0" t="n">
-        <v>-0.005279</v>
+        <v>-0.071354</v>
       </c>
       <c r="G46" s="0" t="n">
-        <v>0.142779</v>
+        <v>-0.125028</v>
       </c>
       <c r="H46" s="0" t="n">
-        <v>0.990955</v>
+        <v>0.989705</v>
       </c>
       <c r="I46" s="0" t="n">
-        <v>23.79402</v>
+        <v>9.232149</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3917,83 +3917,83 @@
         <v>32</v>
       </c>
       <c r="F49" s="0" t="n">
-        <v>-0.650807</v>
+        <v>0.523656</v>
       </c>
       <c r="G49" s="0" t="n">
-        <v>0.752774</v>
+        <v>-0.852103</v>
       </c>
       <c r="H49" s="0" t="n">
-        <v>-0.125083</v>
+        <v>0.016146</v>
       </c>
       <c r="I49" s="0" t="n">
-        <v>572.784851</v>
+        <v>40.158855</v>
       </c>
       <c r="K49" s="0" t="n">
-        <f aca="false">COS(G50) - SIN(H50) + SIN(G51) + COS(H51)</f>
-        <v>1.43396060208831</v>
+        <f aca="false"> (COS(G50) - SIN(H50) + SIN(G51) + COS(H51)) / PI()</f>
+        <v>0.381010879923099</v>
       </c>
       <c r="L49" s="0" t="n">
-        <f aca="false">COS(F49) + SIN(H49) - SIN(F51) + COS(H51)</f>
-        <v>1.30214184943309</v>
+        <f aca="false"> (COS(F49) + SIN(H49) - SIN(F51) + COS(H51)) / PI()</f>
+        <v>0.500453250450588</v>
       </c>
       <c r="M49" s="0" t="n">
-        <f aca="false">COS(F49) - SIN(G49) + SIN(F50) + COS(G50)</f>
-        <v>0.216806550373813</v>
+        <f aca="false"> (COS(F49) - SIN(G49) + SIN(F50) + COS(G50)) / PI()</f>
+        <v>1.02870821036555</v>
       </c>
       <c r="O49" s="0" t="n">
-        <f aca="false">I49</f>
-        <v>572.784851</v>
+        <f aca="false"> I49</f>
+        <v>40.158855</v>
       </c>
       <c r="P49" s="0" t="n">
-        <f aca="false">I50</f>
-        <v>4.02</v>
+        <f aca="false"> I50</f>
+        <v>-353.890869</v>
       </c>
       <c r="Q49" s="0" t="n">
-        <f aca="false">I51</f>
-        <v>20.255424</v>
+        <f aca="false"> I51</f>
+        <v>23.182028</v>
       </c>
       <c r="S49" s="0" t="n">
-        <f aca="false">F49</f>
-        <v>-0.650807</v>
+        <f aca="false"> F49</f>
+        <v>0.523656</v>
       </c>
       <c r="T49" s="0" t="n">
-        <f aca="false">G50</f>
-        <v>-0.656726</v>
+        <f aca="false"> G50</f>
+        <v>0.519553</v>
       </c>
       <c r="U49" s="0" t="n">
-        <f aca="false">H51</f>
-        <v>0.993538</v>
+        <f aca="false"> H51</f>
+        <v>0.987987</v>
       </c>
       <c r="W49" s="0" t="n">
-        <v>20.711356</v>
+        <v>14.841331</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F50" s="0" t="n">
-        <v>-0.757515</v>
+        <v>0.840651</v>
       </c>
       <c r="G50" s="0" t="n">
-        <v>-0.656726</v>
+        <v>0.519553</v>
       </c>
       <c r="H50" s="0" t="n">
-        <v>-0.004944</v>
+        <v>0.154678</v>
       </c>
       <c r="I50" s="0" t="n">
-        <v>4.02</v>
+        <v>-353.890869</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F51" s="0" t="n">
-        <v>-0.08568</v>
+        <v>-0.140165</v>
       </c>
       <c r="G51" s="0" t="n">
-        <v>0.09142</v>
+        <v>-0.067421</v>
       </c>
       <c r="H51" s="0" t="n">
-        <v>0.993538</v>
+        <v>0.987987</v>
       </c>
       <c r="I51" s="0" t="n">
-        <v>20.255424</v>
+        <v>23.182028</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4018,83 +4018,83 @@
         <v>34</v>
       </c>
       <c r="F54" s="0" t="n">
-        <v>-0.146911</v>
+        <v>0.03928</v>
       </c>
       <c r="G54" s="0" t="n">
-        <v>-0.984625</v>
+        <v>-0.994418</v>
       </c>
       <c r="H54" s="0" t="n">
-        <v>0.125225</v>
+        <v>-0.10122</v>
       </c>
       <c r="I54" s="0" t="n">
-        <v>4.781213</v>
+        <v>228.471268</v>
       </c>
       <c r="K54" s="0" t="n">
-        <f aca="false">COS(G55) - SIN(H55) + SIN(G56) + COS(H56)</f>
-        <v>1.68250494040814</v>
+        <f aca="false"> (COS(G55) - SIN(H55) + SIN(G56) + COS(H56)) / PI()</f>
+        <v>0.4322064473861</v>
       </c>
       <c r="L54" s="0" t="n">
-        <f aca="false">COS(F54) + SIN(H54) - SIN(F56) + COS(H56)</f>
-        <v>1.61293616911714</v>
+        <f aca="false"> (COS(F54) + SIN(H54) - SIN(F56) + COS(H56)) / PI()</f>
+        <v>0.486184485935403</v>
       </c>
       <c r="M54" s="0" t="n">
-        <f aca="false">COS(F54) - SIN(G54) + SIN(F55) + COS(G55)</f>
-        <v>3.64714701659245</v>
+        <f aca="false"> (COS(F54) - SIN(G54) + SIN(F55) + COS(G55)) / PI()</f>
+        <v>1.17029886855501</v>
       </c>
       <c r="O54" s="0" t="n">
-        <f aca="false">I54</f>
-        <v>4.781213</v>
+        <f aca="false"> I54</f>
+        <v>228.471268</v>
       </c>
       <c r="P54" s="0" t="n">
-        <f aca="false">I55</f>
-        <v>-189.964249</v>
+        <f aca="false"> I55</f>
+        <v>-326.764984</v>
       </c>
       <c r="Q54" s="0" t="n">
-        <f aca="false">I56</f>
-        <v>19.294014</v>
+        <f aca="false"> I56</f>
+        <v>9.133189</v>
       </c>
       <c r="S54" s="0" t="n">
-        <f aca="false">F54</f>
-        <v>-0.146911</v>
+        <f aca="false"> F54</f>
+        <v>0.03928</v>
       </c>
       <c r="T54" s="0" t="n">
-        <f aca="false">G55</f>
-        <v>-0.152018</v>
+        <f aca="false"> G55</f>
+        <v>0.03065</v>
       </c>
       <c r="U54" s="0" t="n">
-        <f aca="false">H56</f>
-        <v>0.993249</v>
+        <f aca="false"> H56</f>
+        <v>0.991378</v>
       </c>
       <c r="W54" s="0" t="n">
-        <v>17.666445</v>
+        <v>12.612013</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F55" s="0" t="n">
-        <v>0.990658</v>
+        <v>0.996181</v>
       </c>
       <c r="G55" s="0" t="n">
-        <v>-0.152018</v>
+        <v>0.03065</v>
       </c>
       <c r="H55" s="0" t="n">
-        <v>-0.028698</v>
+        <v>0.085366</v>
       </c>
       <c r="I55" s="0" t="n">
-        <v>-189.964249</v>
+        <v>-326.764984</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F56" s="0" t="n">
-        <v>0.047178</v>
+        <v>-0.081766</v>
       </c>
       <c r="G56" s="0" t="n">
-        <v>0.119658</v>
+        <v>-0.104177</v>
       </c>
       <c r="H56" s="0" t="n">
-        <v>0.993249</v>
+        <v>0.991378</v>
       </c>
       <c r="I56" s="0" t="n">
-        <v>19.294014</v>
+        <v>9.133189</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>